<commit_message>
parse ingredients from excel file
</commit_message>
<xml_diff>
--- a/DietMenu.Core/tests/SilentMike.DietMenu.Core.InfrastructureTests/Ingredients.xlsx
+++ b/DietMenu.Core/tests/SilentMike.DietMenu.Core.InfrastructureTests/Ingredients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ComplexCarbohydrate" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
   <si>
     <t xml:space="preserve">Nazwa</t>
   </si>
@@ -46,13 +46,25 @@
     <t xml:space="preserve">g</t>
   </si>
   <si>
+    <t xml:space="preserve">46E7473C-9072-9CFD-3ED7-485AF9998E99</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bataty</t>
   </si>
   <si>
+    <t xml:space="preserve">5CB3DB36-8733-1EBE-56AF-E7CD359A1499</t>
+  </si>
+  <si>
     <t xml:space="preserve">Agrest</t>
   </si>
   <si>
+    <t xml:space="preserve">692D8FD2-6E75-4827-2A2B-7276E17E2867</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ananas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52AD38A0-2C24-2B34-750B-CDD978015802</t>
   </si>
   <si>
     <t xml:space="preserve">Cielęcina (udziec)</t>
@@ -307,16 +319,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -333,65 +349,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="40.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="str">
-        <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4))</f>
-        <v>26996BEA-9973-54D9-3A39-296170521786</v>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>4.1</v>
       </c>
-      <c r="D3" s="0" t="str">
-        <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4))</f>
-        <v>8BD03DAB-025B-3F5A-03A3-6D67F1DB31B9</v>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -448,65 +462,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="D2:D3 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="40.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>2.3</v>
       </c>
-      <c r="D2" s="0" t="str">
-        <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4))</f>
-        <v>86B194C9-1F48-29B8-A554-8304C9020CA4</v>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>1.8</v>
       </c>
-      <c r="D3" s="0" t="str">
-        <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4))</f>
-        <v>02E6F65A-62E4-2E6F-70A8-8A8AF6E79BEE</v>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -563,29 +575,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
+      <selection pane="topLeft" activeCell="I37" activeCellId="1" sqref="D2:D3 I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -634,29 +646,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I43" activeCellId="0" sqref="I43"/>
+      <selection pane="topLeft" activeCell="I43" activeCellId="1" sqref="D2:D3 I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -711,646 +723,646 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U57" activeCellId="0" sqref="U57"/>
+      <selection pane="topLeft" activeCell="U57" activeCellId="1" sqref="D2:D3 U57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="0" t="n">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="0" t="n">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="0" t="n">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="0" t="n">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="0" t="n">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="n">
         <v>1.3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="0" t="n">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="0" t="n">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="0" t="n">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="0" t="n">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="0" t="n">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="n">
         <v>1.3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="0" t="n">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="n">
         <v>1.4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="0" t="n">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="0" t="n">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="0" t="n">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="0" t="n">
+      <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="0" t="n">
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="0" t="n">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="0" t="n">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="0" t="n">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="0" t="n">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="0" t="n">
+      <c r="A32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="0" t="n">
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="n">
         <v>2.2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="0" t="n">
+      <c r="A34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="n">
         <v>1.7</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="0" t="n">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="n">
         <v>1.7</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="0" t="n">
+      <c r="A36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="0" t="n">
+      <c r="A37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1" t="n">
         <v>1.8</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="0" t="n">
+      <c r="A38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="n">
         <v>2.1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="0" t="n">
+      <c r="A39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1" t="n">
         <v>2.2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="0" t="n">
+      <c r="A40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="0" t="n">
+      <c r="A41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="0" t="n">
+      <c r="A42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1" t="n">
         <v>6.2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="0" t="n">
+      <c r="A43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="0" t="n">
+      <c r="A44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="n">
         <v>1.7</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="0" t="n">
+      <c r="A45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="0" t="n">
+      <c r="A46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="0" t="n">
+      <c r="A47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="0" t="n">
+      <c r="A48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="0" t="n">
+      <c r="A49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="0" t="n">
+      <c r="A50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="0" t="n">
+      <c r="A51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="1" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="0" t="n">
+      <c r="A52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="0" t="n">
+      <c r="A53" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1" t="n">
         <v>1.3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="0" t="n">
+      <c r="A54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="0" t="n">
+      <c r="A55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="0" t="n">
+      <c r="A56" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="0" t="n">
+      <c r="A57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="1" t="n">
         <v>1.9</v>
       </c>
     </row>
@@ -1366,29 +1378,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
+      <selection pane="topLeft" activeCell="G44" activeCellId="1" sqref="D2:D3 G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1444,30 +1456,30 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="D2:D3 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>